<commit_message>
adding religion property and health reasons (for reason of migration)
</commit_message>
<xml_diff>
--- a/xforms/xlsforms/in_migration.xlsx
+++ b/xforms/xlsforms/in_migration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25605" yWindow="-195" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
+    <workbookView xWindow="25605" yWindow="-195" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="178">
   <si>
     <t>type</t>
   </si>
@@ -520,6 +520,36 @@
   </si>
   <si>
     <t>. &lt;= today() and . &gt; {earliestDate}</t>
+  </si>
+  <si>
+    <t>religion</t>
+  </si>
+  <si>
+    <t>Christian Orthodox</t>
+  </si>
+  <si>
+    <t>Christian Catholic</t>
+  </si>
+  <si>
+    <t>Muslim</t>
+  </si>
+  <si>
+    <t>Judaism</t>
+  </si>
+  <si>
+    <t>Traditional faith</t>
+  </si>
+  <si>
+    <t>select_one religion</t>
+  </si>
+  <si>
+    <t>Religion</t>
+  </si>
+  <si>
+    <t>HEALTH_REASON</t>
+  </si>
+  <si>
+    <t>Health Reasons</t>
   </si>
 </sst>
 </file>
@@ -1705,13 +1735,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R89"/>
+  <dimension ref="A1:R90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R5" sqref="R5"/>
+      <selection pane="bottomRight" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2199,91 +2229,91 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+        <v>174</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>175</v>
+      </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
-      <c r="I22" s="4"/>
-    </row>
-    <row r="23" spans="1:13" s="16" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A23" s="16" t="s">
+      <c r="I22" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="I23" s="4"/>
+    </row>
+    <row r="24" spans="1:13" s="16" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A24" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B24" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C24" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="D23" s="16" t="s">
+      <c r="D24" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="G23" s="16" t="s">
+      <c r="G24" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="H23" s="16" t="s">
+      <c r="H24" s="16" t="s">
         <v>157</v>
       </c>
-      <c r="I23" s="17" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" s="16" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A24" s="16" t="s">
+      <c r="I24" s="17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" s="16" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A25" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B25" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="D24" s="16" t="s">
+      <c r="D25" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="I24" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="L24" s="16" t="s">
+      <c r="I25" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="L25" s="16" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="I25" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="L25" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
@@ -2291,19 +2321,22 @@
       <c r="I26" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L26" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>71</v>
+        <v>67</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
@@ -2311,22 +2344,19 @@
       <c r="I27" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="L27" s="5" t="s">
-        <v>112</v>
-      </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>156</v>
+        <v>71</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
@@ -2335,21 +2365,21 @@
         <v>1</v>
       </c>
       <c r="L28" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>134</v>
+        <v>21</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>146</v>
+        <v>72</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>144</v>
+        <v>67</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>156</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
@@ -2358,21 +2388,21 @@
         <v>1</v>
       </c>
       <c r="L29" s="5" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
@@ -2380,32 +2410,46 @@
       <c r="I30" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" s="5" t="s">
+      <c r="L30" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="I31" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B32" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C32" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D32" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="M31" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
+      <c r="M32" s="5" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
@@ -2415,7 +2459,6 @@
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
-      <c r="I33" s="3"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
@@ -2445,6 +2488,7 @@
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
+      <c r="I36" s="3"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
@@ -2454,19 +2498,25 @@
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
-      <c r="I37" s="3"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I41" s="3"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="I38" s="3"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I42" s="3"/>
     </row>
-    <row r="50" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I50" s="3"/>
-    </row>
-    <row r="58" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I58" s="3"/>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I43" s="3"/>
+    </row>
+    <row r="51" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I51" s="3"/>
     </row>
     <row r="59" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I59" s="3"/>
@@ -2480,8 +2530,8 @@
     <row r="62" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I62" s="3"/>
     </row>
-    <row r="79" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I79" s="3"/>
+    <row r="63" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I63" s="3"/>
     </row>
     <row r="80" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I80" s="3"/>
@@ -2496,7 +2546,6 @@
       <c r="I83" s="3"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A84" s="3"/>
       <c r="I84" s="3"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
@@ -2508,10 +2557,14 @@
       <c r="I86" s="3"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A87" s="3"/>
       <c r="I87" s="3"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I89" s="3"/>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I88" s="3"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I90" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2521,10 +2574,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2681,13 +2734,13 @@
         <v>66</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>85</v>
+        <v>176</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>102</v>
+        <v>177</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>85</v>
+        <v>177</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -2695,13 +2748,13 @@
         <v>66</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>133</v>
+        <v>85</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>132</v>
+        <v>102</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>132</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -2709,27 +2762,27 @@
         <v>66</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>86</v>
+        <v>133</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>86</v>
+        <v>132</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>93</v>
+        <v>103</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -2737,13 +2790,13 @@
         <v>69</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -2751,13 +2804,13 @@
         <v>69</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -2765,13 +2818,13 @@
         <v>69</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -2779,41 +2832,41 @@
         <v>69</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="13">
-        <v>888</v>
+      <c r="B19" s="13" t="s">
+        <v>91</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>138</v>
+        <v>69</v>
+      </c>
+      <c r="B20" s="13">
+        <v>888</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>137</v>
+        <v>109</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>137</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -2821,13 +2874,13 @@
         <v>136</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -2835,13 +2888,13 @@
         <v>136</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>143</v>
+        <v>139</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -2849,27 +2902,27 @@
         <v>136</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="B24" s="13">
-        <v>1</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>150</v>
+        <v>136</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -2877,13 +2930,13 @@
         <v>149</v>
       </c>
       <c r="B25" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -2891,50 +2944,98 @@
         <v>149</v>
       </c>
       <c r="B26" s="13">
+        <v>2</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="B27" s="13">
         <v>3</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C27" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D27" s="14" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="12"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-    </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="12"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
+      <c r="A28" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="B28" s="13">
+        <v>1</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="12"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
+      <c r="A29" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="B29" s="13">
+        <v>2</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="12"/>
-      <c r="B30" s="13"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
+      <c r="A30" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="B30" s="13">
+        <v>3</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="12"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
+      <c r="A31" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="B31" s="13">
+        <v>4</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="12"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
+      <c r="A32" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="B32" s="13">
+        <v>5</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="12"/>
@@ -3002,13 +3103,13 @@
       <c r="C43" s="14"/>
       <c r="D43" s="14"/>
     </row>
-    <row r="44" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="12"/>
       <c r="B44" s="13"/>
       <c r="C44" s="14"/>
       <c r="D44" s="14"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="15"/>
+    <row r="45" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B45" s="13"/>
       <c r="C45" s="14"/>
       <c r="D45" s="14"/>
@@ -3156,6 +3257,12 @@
       <c r="B69" s="13"/>
       <c r="C69" s="14"/>
       <c r="D69" s="14"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="15"/>
+      <c r="B70" s="13"/>
+      <c r="C70" s="14"/>
+      <c r="D70" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Fixed small problems with InMigration and Visit XLSForm and updated the XML for those
</commit_message>
<xml_diff>
--- a/xforms/xlsforms/in_migration.xlsx
+++ b/xforms/xlsforms/in_migration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25605" yWindow="-195" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="25605" yWindow="-195" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -519,9 +519,6 @@
     <t>earliestDate</t>
   </si>
   <si>
-    <t>. &lt;= today() and . &gt; {earliestDate}</t>
-  </si>
-  <si>
     <t>religion</t>
   </si>
   <si>
@@ -550,6 +547,9 @@
   </si>
   <si>
     <t>Health Reasons</t>
+  </si>
+  <si>
+    <t>. &lt;= today() and . &gt; ${earliestDate}</t>
   </si>
 </sst>
 </file>
@@ -1737,11 +1737,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R90"/>
   <sheetViews>
-    <sheetView zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D22" sqref="D22"/>
+      <selection pane="bottomRight" activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2229,16 +2229,16 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>175</v>
-      </c>
       <c r="D22" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -2276,7 +2276,7 @@
         <v>62</v>
       </c>
       <c r="G24" s="16" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="H24" s="16" t="s">
         <v>157</v>
@@ -2576,7 +2576,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
@@ -2734,13 +2734,13 @@
         <v>66</v>
       </c>
       <c r="B11" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="C11" s="14" t="s">
         <v>176</v>
       </c>
-      <c r="C11" s="14" t="s">
-        <v>177</v>
-      </c>
       <c r="D11" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -2969,72 +2969,72 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="B28" s="13">
+        <v>1</v>
+      </c>
+      <c r="C28" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="B28" s="13">
-        <v>1</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>169</v>
-      </c>
       <c r="D28" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B29" s="13">
         <v>2</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B30" s="13">
         <v>3</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B31" s="13">
         <v>4</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B32" s="13">
         <v>5</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>